<commit_message>
Eliminado curso básico de logueo al sistema
</commit_message>
<xml_diff>
--- a/CU01 Administracion de Supervisores.xlsx
+++ b/CU01 Administracion de Supervisores.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="195" windowWidth="20115" windowHeight="7875"/>
   </bookViews>
   <sheets>
     <sheet name="Admin Sup" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Revisor</t>
   </si>
@@ -77,49 +77,7 @@
 d - El actor hace clic en el botón "Ver" en algún registro del listado de Ventas</t>
   </si>
   <si>
-    <t>Ver Telemarketer, paso 3.a</t>
-  </si>
-  <si>
-    <t>Ver Oportunidad, paso 3.b</t>
-  </si>
-  <si>
-    <t>Ver Campaña, paso 3.c</t>
-  </si>
-  <si>
-    <t>Ver Venta, paso 3.d</t>
-  </si>
-  <si>
-    <t>El sistema muestra el formulario "Iniciar Sesion" con los campos: Usuario y Contraseña; y los botones "Aceptar" y "Cancelar"</t>
-  </si>
-  <si>
-    <t>El actor ingresa usuario y contraseña.</t>
-  </si>
-  <si>
-    <t>El actor hace click en el botón "Aceptar"</t>
-  </si>
-  <si>
-    <t>3.1 El actor hace click en el botón "Cancelar".</t>
-  </si>
-  <si>
-    <t>3.2 El sistema termina su ejecución.</t>
-  </si>
-  <si>
-    <t>4.1 El sistema muestra un mensaje informando "Usuario y/o contraseña incorrecta", retornando al formulario "Iniciar Sesion"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El sistema valida el usuario y el grupo al que pertenece y muestra el formulario Administración de supervisores la cual presenta:
-*Listado de telemarketers asignados al mismo grupo que el supervisor, con botón "Ver" en cada uno de los registros.
-*Listado de oportunidades asignadas al mismo grupo que el supervisor, con botón "Ver" en cada uno de los registros.
-*Listado de campañas asignadas al mismo grupo que el supervisor, con botón "Ver" en cada uno de los registros.
-*Listado de ventas asignadas al mismo grupo que el supervisor, con botón "Ver" en cada uno de los registros.
-</t>
-  </si>
-  <si>
     <t>El actor inició sesión en el sistema, se completó el formulario con toda la información correspondiente al mismo.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El usuario debe pertenecer al tipo "Supervisores".
-</t>
   </si>
   <si>
     <t xml:space="preserve">El actor accede al formulario Administración de Supervisores donde puede:
@@ -128,6 +86,29 @@
 *Ver listado y detalle de las campañas asignadas al mismo grupo que el actor.
 *Ver listado y detalle de las ventas realizadas por el mismo grupo que el actor.
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema muestra el formulario Administración de supervisores la cual presenta:
+*Listado de telemarketers asignados al mismo grupo que el supervisor, con botón "Ver" en cada uno de los registros.
+*Listado de oportunidades asignadas al mismo grupo que el supervisor, con botón "Ver" en cada uno de los registros.
+*Listado de campañas asignadas al mismo grupo que el supervisor, con botón "Ver" en cada uno de los registros.
+*Listado de ventas asignadas al mismo grupo que el supervisor, con botón "Ver" en cada uno de los registros.
+</t>
+  </si>
+  <si>
+    <t>Ver Telemarketer, paso 2.a</t>
+  </si>
+  <si>
+    <t>Ver Oportunidad, paso 2.b</t>
+  </si>
+  <si>
+    <t>Ver Campaña, paso 2.c</t>
+  </si>
+  <si>
+    <t>Ver Venta, paso 2.d</t>
+  </si>
+  <si>
+    <t>El usuario debe pertenecer al tipo de Usuario "Supervisor".</t>
   </si>
 </sst>
 </file>
@@ -325,11 +306,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -381,10 +359,6 @@
     </xf>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -703,223 +677,180 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="66.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="12"/>
-      <c r="B1" s="13" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="23">
+      <c r="C1" s="21">
         <v>42890</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="24"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="22"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="24"/>
+      <c r="C5" s="22"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="25"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:5" ht="129" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="5"/>
+      <c r="B7" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="5"/>
+      <c r="B9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="17" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>1</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" ht="102" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>2</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>1</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:3" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>2</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>3</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="1:3" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>4</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:3" ht="102" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>5</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="5"/>
+      <c r="C19" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Se modificó Postcondicion y numero de version
</commit_message>
<xml_diff>
--- a/CU01 Administracion de Supervisores.xlsx
+++ b/CU01 Administracion de Supervisores.xlsx
@@ -22,9 +22,6 @@
     <t>Versión</t>
   </si>
   <si>
-    <t>0001</t>
-  </si>
-  <si>
     <t>Estado</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
 b - El actor hace clic en el botón "Ver" en algún registro del listado de oportunidades.
 c - El actor hace clic en el botón "Ver" en algún registro del listado de campañas.
 d - El actor hace clic en el botón "Ver" en algún registro del listado de Ventas</t>
-  </si>
-  <si>
-    <t>El actor inició sesión en el sistema, se completó el formulario con toda la información correspondiente al mismo.</t>
   </si>
   <si>
     <t xml:space="preserve">El actor accede al formulario Administración de Supervisores donde puede:
@@ -109,6 +103,12 @@
   </si>
   <si>
     <t>El usuario debe pertenecer al tipo de Usuario "Supervisor".</t>
+  </si>
+  <si>
+    <t>0002</t>
+  </si>
+  <si>
+    <t>Se completó el formulario con toda la información correspondiente al actor</t>
   </si>
 </sst>
 </file>
@@ -681,7 +681,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,7 +694,7 @@
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="11"/>
       <c r="B1" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="21">
         <v>42890</v>
@@ -704,10 +704,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="4"/>
@@ -715,10 +715,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="4"/>
@@ -736,49 +736,49 @@
         <v>1</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C5" s="22"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="20" t="s">
         <v>3</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>4</v>
       </c>
       <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:5" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="4"/>
@@ -786,34 +786,34 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="4"/>
@@ -823,7 +823,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" s="4"/>
     </row>
@@ -832,23 +832,23 @@
         <v>2</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="4"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C19" s="4"/>
     </row>

</xml_diff>